<commit_message>
ft: codigo asm copy
se agrega el copy para el ultimo ejemplo de los ejercicios
</commit_message>
<xml_diff>
--- a/ProyectoSoftwareSistemas/bin/Debug/ArchivoIntermedio.xlsx
+++ b/ProyectoSoftwareSistemas/bin/Debug/ArchivoIntermedio.xlsx
@@ -40,18 +40,15 @@
     <x:t>Errores</x:t>
   </x:si>
   <x:si>
-    <x:t>0000</x:t>
-  </x:si>
-  <x:si>
-    <x:t>EJER1</x:t>
+    <x:t>1000</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COPY</x:t>
   </x:si>
   <x:si>
     <x:t>START</x:t>
   </x:si>
   <x:si>
-    <x:t>0</x:t>
-  </x:si>
-  <x:si>
     <x:t>-</x:t>
   </x:si>
   <x:si>
@@ -61,166 +58,94 @@
     <x:t/>
   </x:si>
   <x:si>
-    <x:t>LDX</x:t>
-  </x:si>
-  <x:si>
-    <x:t>#5</x:t>
+    <x:t>FIRST</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RETADR</x:t>
   </x:si>
   <x:si>
     <x:t>3</x:t>
   </x:si>
   <x:si>
+    <x:t>Simple</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1003</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CLOOP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+JSUB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RDREC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1007</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LDA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LENGTH</x:t>
+  </x:si>
+  <x:si>
+    <x:t>100A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CLEAR</x:t>
+  </x:si>
+  <x:si>
+    <x:t>X</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>--</x:t>
+  </x:si>
+  <x:si>
+    <x:t>100C</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LDT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>#3</x:t>
+  </x:si>
+  <x:si>
     <x:t>Inmediato</x:t>
   </x:si>
   <x:si>
-    <x:t>0003</x:t>
-  </x:si>
-  <x:si>
-    <x:t>HIO</x:t>
+    <x:t>100F</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RSUB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1012</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RESW</x:t>
   </x:si>
   <x:si>
     <x:t>1</x:t>
   </x:si>
   <x:si>
-    <x:t>0004</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+LDB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>#TABLE2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0008</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>@COUNT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Indirecto</x:t>
-  </x:si>
-  <x:si>
-    <x:t>000B</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CLEAR</x:t>
-  </x:si>
-  <x:si>
-    <x:t>A</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>--</x:t>
-  </x:si>
-  <x:si>
-    <x:t>000D</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BASE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TABLE2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ADDR</x:t>
-  </x:si>
-  <x:si>
-    <x:t>X,A</x:t>
-  </x:si>
-  <x:si>
-    <x:t>000F</x:t>
-  </x:si>
-  <x:si>
-    <x:t>LOOP</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ADD</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TABLE,X</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Indexado</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0012</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+STA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TOTAL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Simple</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0016</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RSUB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0019</x:t>
-  </x:si>
-  <x:si>
-    <x:t>COUNT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RESB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12H</x:t>
-  </x:si>
-  <x:si>
-    <x:t>002B</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SHIFTL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>X,2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>002D</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TABLE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RESW</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>004B</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BYTE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C'TEST'</x:t>
-  </x:si>
-  <x:si>
-    <x:t>004F</x:t>
+    <x:t>1015</x:t>
   </x:si>
   <x:si>
     <x:t>WORD</x:t>
   </x:si>
   <x:si>
-    <x:t>16</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0052</x:t>
+    <x:t>1018</x:t>
   </x:si>
   <x:si>
     <x:t>END</x:t>
@@ -574,7 +499,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:H18"/>
+  <x:dimension ref="A1:H11"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -620,16 +545,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="F2" s="0" t="s">
+      <x:c r="G2" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="G2" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
       <x:c r="H2" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
@@ -655,7 +580,7 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="H3" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:8">
@@ -666,22 +591,22 @@
         <x:v>19</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E4" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F4" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="G4" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="H4" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:8">
@@ -689,25 +614,25 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="F5" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G5" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="H5" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -715,25 +640,25 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="F6" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="G6" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="H6" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:8">
@@ -741,25 +666,25 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="E7" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="F7" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G7" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="H7" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:8">
@@ -767,25 +692,25 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="E8" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="F8" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G8" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
       <x:c r="H8" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:8">
@@ -793,25 +718,25 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="E9" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="F9" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="G9" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="H9" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:8">
@@ -819,25 +744,25 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
         <x:v>42</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="F10" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="G10" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="H10" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -845,207 +770,25 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="D11" s="0" t="s">
-        <x:v>46</x:v>
-      </x:c>
-      <x:c r="E11" s="0" t="s">
-        <x:v>47</x:v>
-      </x:c>
       <x:c r="F11" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="G11" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="H11" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:8">
-      <x:c r="A12" s="0">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="B12" s="0" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="C12" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="D12" s="0" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="E12" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="F12" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="G12" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="H12" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:8">
-      <x:c r="A13" s="0">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B13" s="0" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="C13" s="0" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="D13" s="0" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="E13" s="0" t="s">
-        <x:v>54</x:v>
-      </x:c>
-      <x:c r="F13" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="G13" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="H13" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:8">
-      <x:c r="A14" s="0">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="B14" s="0" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="C14" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="D14" s="0" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="E14" s="0" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="F14" s="0" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="G14" s="0" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="H14" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:8">
-      <x:c r="A15" s="0">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="B15" s="0" t="s">
-        <x:v>58</x:v>
-      </x:c>
-      <x:c r="C15" s="0" t="s">
-        <x:v>59</x:v>
-      </x:c>
-      <x:c r="D15" s="0" t="s">
-        <x:v>60</x:v>
-      </x:c>
-      <x:c r="E15" s="0" t="s">
-        <x:v>61</x:v>
-      </x:c>
-      <x:c r="F15" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="G15" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="H15" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:8">
-      <x:c r="A16" s="0">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="B16" s="0" t="s">
-        <x:v>62</x:v>
-      </x:c>
-      <x:c r="C16" s="0" t="s">
-        <x:v>37</x:v>
-      </x:c>
-      <x:c r="D16" s="0" t="s">
-        <x:v>63</x:v>
-      </x:c>
-      <x:c r="E16" s="0" t="s">
-        <x:v>64</x:v>
-      </x:c>
-      <x:c r="F16" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="G16" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="H16" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:8">
-      <x:c r="A17" s="0">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="B17" s="0" t="s">
-        <x:v>65</x:v>
-      </x:c>
-      <x:c r="C17" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="D17" s="0" t="s">
-        <x:v>66</x:v>
-      </x:c>
-      <x:c r="E17" s="0" t="s">
-        <x:v>67</x:v>
-      </x:c>
-      <x:c r="F17" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="G17" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="H17" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:8">
-      <x:c r="A18" s="0">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="B18" s="0" t="s">
-        <x:v>68</x:v>
-      </x:c>
-      <x:c r="C18" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="D18" s="0" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="E18" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="F18" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="G18" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="H18" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>